<commit_message>
fixed the integration issues
</commit_message>
<xml_diff>
--- a/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
+++ b/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="152">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -56,333 +56,342 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
+    <t xml:space="preserve">Vijay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Initial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tudu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DatePicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place of Birth (State)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DropDown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Security #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">347563874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have a valid driver's license?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver's license #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State of issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona (AZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address (Number, Street, and Apt. #) (No P.O. Box please)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone (HOME/CELL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999-999-9999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone (WORK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vijay@sureify.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is your mailing address different from your home address?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you currently employed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter your occupation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutoSugg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employer name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sureify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employer address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address (Number, Street, and Apt.#)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California (CA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you currently disabled?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you collected disability benefits in the last two years?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Charitable Giving Rider provides for a donation to an IRS section 501(c)(3) qualified charity of your choosing. Election of the rider is available prior to or at issue only. Selection of this Rider does not change your premium. Do you wish to elect the Charitable Giving Rider?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Owner the same as the Proposed Insured?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Payor the same as the Owner?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the Proposed Insured have existing life insurance or annuity contracts in force?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the Proposed Insured have any applications for life insurance now pending?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you intend to replace, discontinue or change any existing life insurance or annuity contracts on the Proposed Insured with the applied-for policy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed At City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City in issue state where application is signed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the past three years has the Proposed Insured or does the Proposed Insured intend in the next two years:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to pilot an aircraft (other than scheduled commercial or corporate aviation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engage in any of the following: sky sports, underwater sports to a depth of greater than 100 feet, climbing sports greater than 5.0 difficulty, motor sport traveling at speeds (in any type vehicle) in excess of 100 miles per hour or bungee jumping, heli-skiing, hang gliding, sky diving, parachuting, BASE jumping?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the Proposed Insured used tobacco products or products containing nicotine in any form (to include cigarettes, electronic cigarettes, cannabis cigarettes, snuff/chew/dip, cigars, pipes, nicotine patch and nicotine gum) in the past 5 years?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the next 12 months, does the Proposed Insured intend to live or travel outside the U.S or Canada?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the last 10 years, has the Proposed Insured:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">been convicted of a felony; convicted of a misdemeanor; or is the Proposed Insured currently on parole or incarcerated in a correctional institution?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">been convicted of operating a vehicle while under the influence of alcohol or drugs; or does the Proposed Insured currently have a revoked or suspended license?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the last three years, has the Proposed Insured plead guilty or been convicted of three or more moving violations?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current height (ft/in)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height (ft)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height (in)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight [lbs]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has your weight changed more than 10 pounds within the past year?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the Proposed Insured currently confined to a hospital, nursing home, psychiatric facility or currently receiving home health care/assisted living care?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the Proposed Insured ever been declined, postponed, or offered rated life or health insurance or been denied a reinstatement, reissue or renewal for life or health insurance?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the past ten years, have you been diagnosed with or treated by a licensed member of the medical profession for any of the following?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease of heart, blood vessels, high blood pressure, heart murmur, coronary artery disease, chest pain, palpitation or other abnormal heart rate or rhythm, or heart attack?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease or disorder of lungs, nose, sinus or throat, including asthma, tuberculosis, emphysema, chronic bronchitis, cough, shortness of breath, or sleep disorder/apnea?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease or disorder of the pancreas, esophagus, stomach or intestinal tract including abdominal pain or internal bleeding, ulcer or jaundice?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease of kidney, urinary bladder, liver or gall bladder, prostate, or protein, blood or sugar in urine?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease or disorder of the brain or nervous system including headache, dizziness, epilepsy or seizures, paralysis, stroke, depression, anxiety or mental illness?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diabetes, thyroid condition or other glandular disorder or gout?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disorder of the skin, lymph glands, muscles, bones, joints, arthritis or back disorder?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disorder of the eye or ear, or any impaired sight or hearing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tumor, cancer, anemia, or blood disorder?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquired Immune Deficiency Syndrome (AIDS), AIDS Related Complex (ARC) or AIDS related conditions?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the Proposed Insured ever:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Been treated or counseled for alcoholism, alcohol abuse or addiction?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used amphetamines, heroin, narcotics, barbiturates, cocaine, hallucinogens, cannabis or any drugs except prescribed by a physician?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had a positive result on a Human Immunodeficiency Virus (HIV) test administered by a member of the medical profession?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other than the above, is the Proposed Insured now under observation or receiving treatment or counseling by a member of the medical profession?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the Proposed Insured have a regular personal physician?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has a biological parent or sibling of the Proposed Insured died or been diagnosed or treated by a licensed member of the medical profession with heart disease, stroke, or cancer prior to the age of 60?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneficiaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary beneficiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary beneficiary 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationship to Proposed Insured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneficiary Social Security Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address (Number, Street)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contingent beneficiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"id":"TermLife","label":"Level Term Life"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"id":"TenYearTerm","label":"10 Year Level"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"id":"IncomeReplacement","label":"Income Replacement"}]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yughander</t>
   </si>
   <si>
-    <t xml:space="preserve">Middle Initial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Akkunuru</t>
   </si>
   <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DatePicker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place of Birth (State)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DropDown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arizona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Security #</t>
+    <t xml:space="preserve">{"id":"Male","label":"Male"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"id":"ArizonaAZ","label":"Arizona (AZ)"}</t>
   </si>
   <si>
     <t xml:space="preserve">347-56-3874</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you have a valid driver's license?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driver's license #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State of issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arizona (AZ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SampleTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Address (Number, Street, and Apt. #) (No P.O. Box please)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone (HOME/CELL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">999-999-9999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone (WORK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vijay@sureify.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is your mailing address different from your home address?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are you currently employed?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter your occupation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AutoSugg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employer name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sureify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employer address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address (Number, Street, and Apt.#)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California (CA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are you currently disabled?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have you collected disability benefits in the last two years?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Charitable Giving Rider provides for a donation to an IRS section 501(c)(3) qualified charity of your choosing. Election of the rider is available prior to or at issue only. Selection of this Rider does not change your premium. Do you wish to elect the Charitable Giving Rider?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Owner the same as the Proposed Insured?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Payor the same as the Owner?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the Proposed Insured have existing life insurance or annuity contracts in force?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the Proposed Insured have any applications for life insurance now pending?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you intend to replace, discontinue or change any existing life insurance or annuity contracts on the Proposed Insured with the applied-for policy?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signed At City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City in issue state where application is signed:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the past three years has the Proposed Insured or does the Proposed Insured intend in the next two years:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to pilot an aircraft (other than scheduled commercial or corporate aviation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engage in any of the following: sky sports, underwater sports to a depth of greater than 100 feet, climbing sports greater than 5.0 difficulty, motor sport traveling at speeds (in any type vehicle) in excess of 100 miles per hour or bungee jumping, heli-skiing, hang gliding, sky diving, parachuting, BASE jumping?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the Proposed Insured used tobacco products or products containing nicotine in any form (to include cigarettes, electronic cigarettes, cannabis cigarettes, snuff/chew/dip, cigars, pipes, nicotine patch and nicotine gum) in the past 5 years?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the next 12 months, does the Proposed Insured intend to live or travel outside the U.S or Canada?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the last 10 years, has the Proposed Insured:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">been convicted of a felony; convicted of a misdemeanor; or is the Proposed Insured currently on parole or incarcerated in a correctional institution?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">been convicted of operating a vehicle while under the influence of alcohol or drugs; or does the Proposed Insured currently have a revoked or suspended license?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the last three years, has the Proposed Insured plead guilty or been convicted of three or more moving violations?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current height (ft/in)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">height (ft)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">height (in)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight [lbs]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has your weight changed more than 10 pounds within the past year?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the Proposed Insured currently confined to a hospital, nursing home, psychiatric facility or currently receiving home health care/assisted living care?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the Proposed Insured ever been declined, postponed, or offered rated life or health insurance or been denied a reinstatement, reissue or renewal for life or health insurance?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the past ten years, have you been diagnosed with or treated by a licensed member of the medical profession for any of the following?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disease of heart, blood vessels, high blood pressure, heart murmur, coronary artery disease, chest pain, palpitation or other abnormal heart rate or rhythm, or heart attack?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disease or disorder of lungs, nose, sinus or throat, including asthma, tuberculosis, emphysema, chronic bronchitis, cough, shortness of breath, or sleep disorder/apnea?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disease or disorder of the pancreas, esophagus, stomach or intestinal tract including abdominal pain or internal bleeding, ulcer or jaundice?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disease of kidney, urinary bladder, liver or gall bladder, prostate, or protein, blood or sugar in urine?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disease or disorder of the brain or nervous system including headache, dizziness, epilepsy or seizures, paralysis, stroke, depression, anxiety or mental illness?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetes, thyroid condition or other glandular disorder or gout?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disorder of the skin, lymph glands, muscles, bones, joints, arthritis or back disorder?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disorder of the eye or ear, or any impaired sight or hearing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tumor, cancer, anemia, or blood disorder?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acquired Immune Deficiency Syndrome (AIDS), AIDS Related Complex (ARC) or AIDS related conditions?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the Proposed Insured ever:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Been treated or counseled for alcoholism, alcohol abuse or addiction?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used amphetamines, heroin, narcotics, barbiturates, cocaine, hallucinogens, cannabis or any drugs except prescribed by a physician?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Had a positive result on a Human Immunodeficiency Virus (HIV) test administered by a member of the medical profession?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other than the above, is the Proposed Insured now under observation or receiving treatment or counseling by a member of the medical profession?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the Proposed Insured have a regular personal physician?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has a biological parent or sibling of the Proposed Insured died or been diagnosed or treated by a licensed member of the medical profession with heart disease, stroke, or cancer prior to the age of 60?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beneficiaries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary beneficiary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primary beneficiary 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relationship to Proposed Insured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beneficiary Social Security Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address (Number, Street)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingent beneficiary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"id":"TermLife","label":"Level Term Life"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"id":"TenYearTerm","label":"10 Year Level"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"id":"IncomeReplacement","label":"Income Replacement"}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"id":"Male","label":"Male"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"id":"ArizonaAZ","label":"Arizona (AZ)"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{"id":"Yes","label":"Yes"}</t>
   </si>
   <si>
@@ -404,9 +413,6 @@
     <t xml:space="preserve">[{"id":"PrimaryBeneficiary1","label":"primary beneficiary 1","inferred":false,"addedBySearchVariable":true,"category":"Personal"}]</t>
   </si>
   <si>
-    <t xml:space="preserve">Vijay</t>
-  </si>
-  <si>
     <t xml:space="preserve">{"id":"BrotherRelation","label":"Brother"}</t>
   </si>
   <si>
@@ -428,19 +434,22 @@
     <t xml:space="preserve">State_code</t>
   </si>
   <si>
+    <t xml:space="preserve">Ajay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05.01.1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alaska</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05.01.1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alaska</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AK</t>
   </si>
   <si>
     <t xml:space="preserve">searchString</t>
@@ -488,7 +497,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -510,13 +518,11 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -580,7 +586,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -619,6 +625,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -708,8 +718,8 @@
   </sheetPr>
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C:C"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -767,7 +777,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -789,7 +799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -833,7 +843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -895,7 +905,7 @@
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="10" t="n">
         <v>4637</v>
       </c>
     </row>
@@ -928,7 +938,7 @@
       <c r="B21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="8" t="n">
+      <c r="C21" s="10" t="n">
         <v>95125</v>
       </c>
     </row>
@@ -994,7 +1004,7 @@
       <c r="A28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="8"/>
@@ -1035,7 +1045,7 @@
       <c r="B32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8" t="n">
+      <c r="C32" s="10" t="n">
         <v>3465</v>
       </c>
     </row>
@@ -1068,7 +1078,7 @@
       <c r="B35" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="8" t="n">
+      <c r="C35" s="10" t="n">
         <v>95125</v>
       </c>
     </row>
@@ -1696,7 +1706,7 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1797,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,10 +1841,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1861,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,10 +1874,10 @@
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D11" s="12" t="n">
         <v>32092</v>
       </c>
-      <c r="E11" s="11" t="n">
+      <c r="E11" s="12" t="n">
         <v>32092</v>
       </c>
     </row>
@@ -1885,7 +1895,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,10 +1909,10 @@
         <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,7 +1929,7 @@
         <v>26</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,12 +1963,12 @@
         <v>29</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>113</v>
@@ -1970,7 +1980,7 @@
         <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,7 +2031,7 @@
         <v>29</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,7 +2073,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2100,7 +2110,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2127,7 @@
         <v>26</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,12 +2146,12 @@
       <c r="B28" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2237,7 +2247,7 @@
         <v>52</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,7 +2281,7 @@
         <v>42</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,7 +2298,7 @@
         <v>42</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2315,7 @@
         <v>42</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2332,7 @@
         <v>26</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,7 +2349,7 @@
         <v>26</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,7 +2366,7 @@
         <v>42</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,7 +2383,7 @@
         <v>42</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,7 +2400,7 @@
         <v>42</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2461,7 @@
         <v>42</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2478,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,7 +2495,7 @@
         <v>42</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2512,7 @@
         <v>42</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +2542,7 @@
         <v>42</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2549,7 +2559,7 @@
         <v>42</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,7 +2576,7 @@
         <v>42</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,7 +2664,7 @@
         <v>42</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2681,7 @@
         <v>42</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2688,7 +2698,7 @@
         <v>42</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2715,7 @@
         <v>42</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,7 +2732,7 @@
         <v>42</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,7 +2749,7 @@
         <v>42</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2766,7 @@
         <v>42</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2773,7 +2783,7 @@
         <v>42</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2790,7 +2800,7 @@
         <v>42</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,7 +2817,7 @@
         <v>42</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,7 +2834,7 @@
         <v>42</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2851,7 @@
         <v>42</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,7 +2868,7 @@
         <v>42</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,7 +2885,7 @@
         <v>42</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,7 +2915,7 @@
         <v>42</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,7 +2932,7 @@
         <v>42</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,7 +2949,7 @@
         <v>42</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,7 +2966,7 @@
         <v>42</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,7 +2983,7 @@
         <v>42</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,7 +3000,7 @@
         <v>42</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3012,7 +3022,7 @@
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,7 +3046,7 @@
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,7 +3061,7 @@
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3081,7 +3091,7 @@
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,7 +3103,7 @@
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
-      <c r="E89" s="11" t="n">
+      <c r="E89" s="12" t="n">
         <v>32092</v>
       </c>
     </row>
@@ -3102,7 +3112,7 @@
         <v>106</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -3113,7 +3123,7 @@
         <v>107</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -3124,7 +3134,7 @@
         <v>32</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -3135,7 +3145,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -3146,7 +3156,7 @@
         <v>35</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -3157,7 +3167,7 @@
         <v>108</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -3207,7 +3217,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C:C B9"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3223,10 +3233,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>15</v>
@@ -3235,36 +3245,36 @@
         <v>34</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3286,7 +3296,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C:C A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3301,10 +3311,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>15</v>
@@ -3313,36 +3323,36 @@
         <v>34</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3364,7 +3374,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="C:C A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3376,45 +3386,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>42</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automation is stable till the signup page
</commit_message>
<xml_diff>
--- a/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
+++ b/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="156">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -509,7 +509,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -531,13 +530,11 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -608,7 +605,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -663,6 +660,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -748,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1011,8 +1012,12 @@
       <c r="A23" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="D23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,7 +1437,7 @@
       <c r="D59" s="11"/>
     </row>
     <row r="60" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -1763,7 +1768,9 @@
       <c r="A89" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B89" s="9"/>
+      <c r="B89" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="C89" s="10"/>
       <c r="D89" s="11"/>
     </row>
@@ -1850,7 +1857,7 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="B23:C23 E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2018,10 +2025,10 @@
       <c r="C11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="15" t="n">
         <v>32092</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="15" t="n">
         <v>32092</v>
       </c>
     </row>
@@ -3247,7 +3254,7 @@
       </c>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
-      <c r="E89" s="14" t="n">
+      <c r="E89" s="15" t="n">
         <v>32092</v>
       </c>
     </row>
@@ -3361,7 +3368,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B23:C23 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3440,7 +3447,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B23:C23 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3518,7 +3525,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B23:C23 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
fixed over flow issues, by passed the signature
</commit_message>
<xml_diff>
--- a/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
+++ b/src/main/java/com/lco/qa/testdata/LCO_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="157">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve">Weight [lbs]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
   </si>
   <si>
     <t xml:space="preserve">Has your weight changed more than 10 pounds within the past year?</t>
@@ -509,6 +512,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -530,11 +534,13 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -749,15 +755,15 @@
   </sheetPr>
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23:C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="67.5910931174089"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.1295546558705"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.246963562753"/>
   </cols>
@@ -840,7 +846,7 @@
       </c>
       <c r="D8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -1436,12 +1442,12 @@
       </c>
       <c r="D59" s="11"/>
     </row>
-    <row r="60" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C60" s="10" t="n">
         <v>180</v>
@@ -1450,7 +1456,7 @@
     </row>
     <row r="61" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>17</v>
@@ -1462,7 +1468,7 @@
     </row>
     <row r="62" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>17</v>
@@ -1474,7 +1480,7 @@
     </row>
     <row r="63" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>17</v>
@@ -1486,7 +1492,7 @@
     </row>
     <row r="64" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>17</v>
@@ -1498,7 +1504,7 @@
     </row>
     <row r="65" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>17</v>
@@ -1510,7 +1516,7 @@
     </row>
     <row r="66" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>17</v>
@@ -1522,7 +1528,7 @@
     </row>
     <row r="67" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>17</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="68" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>17</v>
@@ -1546,7 +1552,7 @@
     </row>
     <row r="69" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>17</v>
@@ -1558,7 +1564,7 @@
     </row>
     <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>17</v>
@@ -1570,7 +1576,7 @@
     </row>
     <row r="71" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>17</v>
@@ -1582,7 +1588,7 @@
     </row>
     <row r="72" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>17</v>
@@ -1594,7 +1600,7 @@
     </row>
     <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>17</v>
@@ -1606,7 +1612,7 @@
     </row>
     <row r="74" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>17</v>
@@ -1618,7 +1624,7 @@
     </row>
     <row r="75" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>17</v>
@@ -1630,7 +1636,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>17</v>
@@ -1642,7 +1648,7 @@
     </row>
     <row r="77" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>17</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="78" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>17</v>
@@ -1666,7 +1672,7 @@
     </row>
     <row r="79" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>17</v>
@@ -1678,7 +1684,7 @@
     </row>
     <row r="80" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>17</v>
@@ -1690,7 +1696,7 @@
     </row>
     <row r="81" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>17</v>
@@ -1702,7 +1708,7 @@
     </row>
     <row r="82" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
@@ -1710,7 +1716,7 @@
     </row>
     <row r="83" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
@@ -1718,7 +1724,7 @@
     </row>
     <row r="84" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
@@ -1726,7 +1732,7 @@
     </row>
     <row r="85" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>10</v>
@@ -1736,7 +1742,7 @@
     </row>
     <row r="86" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>22</v>
@@ -1746,7 +1752,7 @@
     </row>
     <row r="87" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>10</v>
@@ -1756,7 +1762,7 @@
     </row>
     <row r="88" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B88" s="9" t="s">
         <v>10</v>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="90" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
@@ -1784,7 +1790,7 @@
     </row>
     <row r="91" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
@@ -1810,7 +1816,7 @@
     </row>
     <row r="95" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
@@ -1818,7 +1824,7 @@
     </row>
     <row r="96" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
@@ -1832,7 +1838,7 @@
     </row>
     <row r="98" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="7"/>
@@ -1857,15 +1863,15 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="B23:C23 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="67.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="68.1295546558705"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.246963562753"/>
   </cols>
   <sheetData>
@@ -1874,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1883,7 +1889,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,12 +1906,12 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,12 +1919,12 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1932,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1939,12 +1945,12 @@
         <v>8</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,16 +1958,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,7 +1975,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>10</v>
@@ -1986,16 +1992,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,7 +2009,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>17</v>
@@ -2012,7 +2018,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2020,7 +2026,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>20</v>
@@ -2037,7 +2043,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>22</v>
@@ -2046,7 +2052,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,16 +2060,16 @@
         <v>24</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,7 +2077,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>17</v>
@@ -2080,7 +2086,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2094,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
@@ -2105,7 +2111,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
@@ -2114,15 +2120,15 @@
         <v>31</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>17</v>
@@ -2131,7 +2137,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,7 +2145,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>10</v>
@@ -2156,7 +2162,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>10</v>
@@ -2173,7 +2179,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>22</v>
@@ -2182,7 +2188,7 @@
         <v>31</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,7 +2196,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>10</v>
@@ -2207,16 +2213,16 @@
         <v>38</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2230,7 @@
         <v>40</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2235,7 +2241,7 @@
         <v>41</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>10</v>
@@ -2252,7 +2258,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>17</v>
@@ -2261,7 +2267,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,7 +2275,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>17</v>
@@ -2278,7 +2284,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,14 +2301,14 @@
         <v>47</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2310,7 +2316,7 @@
         <v>50</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>10</v>
@@ -2327,7 +2333,7 @@
         <v>51</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>10</v>
@@ -2344,7 +2350,7 @@
         <v>53</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2355,7 +2361,7 @@
         <v>54</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>10</v>
@@ -2372,7 +2378,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>10</v>
@@ -2389,7 +2395,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>22</v>
@@ -2398,7 +2404,7 @@
         <v>55</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2406,7 +2412,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>10</v>
@@ -2423,7 +2429,7 @@
         <v>56</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>17</v>
@@ -2432,7 +2438,7 @@
         <v>44</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2446,7 @@
         <v>57</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>17</v>
@@ -2449,7 +2455,7 @@
         <v>44</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2463,7 @@
         <v>58</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>17</v>
@@ -2466,7 +2472,7 @@
         <v>44</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2480,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>17</v>
@@ -2483,7 +2489,7 @@
         <v>27</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,7 +2497,7 @@
         <v>60</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>17</v>
@@ -2500,7 +2506,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +2514,7 @@
         <v>61</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>17</v>
@@ -2517,7 +2523,7 @@
         <v>44</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2531,7 @@
         <v>62</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>17</v>
@@ -2534,7 +2540,7 @@
         <v>44</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2542,7 +2548,7 @@
         <v>63</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>17</v>
@@ -2551,7 +2557,7 @@
         <v>44</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2568,7 +2574,7 @@
         <v>65</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>10</v>
@@ -2603,7 +2609,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>17</v>
@@ -2612,7 +2618,7 @@
         <v>44</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2626,7 @@
         <v>69</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>17</v>
@@ -2629,7 +2635,7 @@
         <v>44</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2643,7 @@
         <v>70</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>17</v>
@@ -2646,7 +2652,7 @@
         <v>44</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,7 +2660,7 @@
         <v>71</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>17</v>
@@ -2663,7 +2669,7 @@
         <v>44</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +2690,7 @@
         <v>73</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>17</v>
@@ -2693,7 +2699,7 @@
         <v>44</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,7 +2707,7 @@
         <v>74</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>17</v>
@@ -2710,7 +2716,7 @@
         <v>44</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,7 +2724,7 @@
         <v>75</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>17</v>
@@ -2727,7 +2733,7 @@
         <v>44</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,7 +2750,7 @@
         <v>77</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2755,7 +2761,7 @@
         <v>78</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>10</v>
@@ -2772,7 +2778,7 @@
         <v>79</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>10</v>
@@ -2789,7 +2795,7 @@
         <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>10</v>
@@ -2803,10 +2809,10 @@
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>17</v>
@@ -2815,15 +2821,15 @@
         <v>44</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>17</v>
@@ -2832,15 +2838,15 @@
         <v>44</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>17</v>
@@ -2849,15 +2855,15 @@
         <v>44</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>17</v>
@@ -2866,15 +2872,15 @@
         <v>44</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>17</v>
@@ -2883,15 +2889,15 @@
         <v>44</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>17</v>
@@ -2900,15 +2906,15 @@
         <v>44</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>17</v>
@@ -2917,15 +2923,15 @@
         <v>44</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>17</v>
@@ -2934,15 +2940,15 @@
         <v>44</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>17</v>
@@ -2951,15 +2957,15 @@
         <v>44</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>17</v>
@@ -2968,15 +2974,15 @@
         <v>44</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>17</v>
@@ -2985,15 +2991,15 @@
         <v>44</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>17</v>
@@ -3002,15 +3008,15 @@
         <v>44</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>17</v>
@@ -3019,15 +3025,15 @@
         <v>44</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>17</v>
@@ -3036,12 +3042,12 @@
         <v>44</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="9" t="s">
@@ -3054,10 +3060,10 @@
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>17</v>
@@ -3066,15 +3072,15 @@
         <v>44</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>17</v>
@@ -3083,15 +3089,15 @@
         <v>44</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>17</v>
@@ -3100,15 +3106,15 @@
         <v>44</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>17</v>
@@ -3117,15 +3123,15 @@
         <v>44</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>17</v>
@@ -3134,15 +3140,15 @@
         <v>44</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>17</v>
@@ -3151,12 +3157,12 @@
         <v>44</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -3165,20 +3171,20 @@
     </row>
     <row r="83" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3187,10 +3193,10 @@
     </row>
     <row r="85" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>10</v>
@@ -3202,25 +3208,25 @@
     </row>
     <row r="86" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>10</v>
@@ -3232,17 +3238,17 @@
     </row>
     <row r="88" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C88" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3250,7 +3256,7 @@
         <v>19</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -3260,10 +3266,10 @@
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
@@ -3271,10 +3277,10 @@
     </row>
     <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
@@ -3285,7 +3291,7 @@
         <v>34</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
@@ -3296,7 +3302,7 @@
         <v>36</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
@@ -3307,7 +3313,7 @@
         <v>37</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
@@ -3315,10 +3321,10 @@
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
@@ -3326,7 +3332,7 @@
     </row>
     <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3342,7 +3348,7 @@
     </row>
     <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3368,26 +3374,26 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B23:C23 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>16</v>
@@ -3396,36 +3402,36 @@
         <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3447,25 +3453,25 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B23:C23 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>16</v>
@@ -3474,36 +3480,36 @@
         <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3525,7 +3531,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B23:C23 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3537,45 +3543,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>